<commit_message>
Implement example AmortizationSchedule with new algorithm
</commit_message>
<xml_diff>
--- a/examples/amortization_schedule.xlsx
+++ b/examples/amortization_schedule.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/murdho/Dropbox (Inbank AS)/shared/portfolio/open-source-payment-schedule/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/murdho/Developer/payment_schedule/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -681,8 +681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:XFD66"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="P42" sqref="P42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2574,7 +2574,7 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="I66" s="11">
+      <c r="I66" s="21">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>

</xml_diff>